<commit_message>
commit all the changes by far
</commit_message>
<xml_diff>
--- a/0322/circumstances.xlsx
+++ b/0322/circumstances.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="896"/>
+    <workbookView xWindow="1760" yWindow="20" windowWidth="23300" windowHeight="14260" tabRatio="971" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="count" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'by year'!$A$1:$C$282</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">count!$A$1:$B$34</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -146,10 +151,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,13 +193,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -189,6 +218,247 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>distracted_year!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>crash_year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>distracted_year!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2005.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2006.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2007.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2008.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2009.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2011.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2012.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>distracted_year!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COUNT(DISTINCT crash_rpt_no)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>distracted_year!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1462.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1537.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1094.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>916.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>777.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>514.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>394.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>213.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>218.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>239.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2101925032"/>
+        <c:axId val="-2125734840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2101925032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2125734840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2125734840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2101925032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,20 +748,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -507,7 +776,7 @@
         <v>20642</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -515,7 +784,7 @@
         <v>7624</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -523,7 +792,7 @@
         <v>5134</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -531,7 +800,7 @@
         <v>4079</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -539,7 +808,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -547,7 +816,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -555,7 +824,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -563,7 +832,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -571,7 +840,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -579,7 +848,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -587,7 +856,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -595,7 +864,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -603,7 +872,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -611,7 +880,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -619,7 +888,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -627,7 +896,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -635,7 +904,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -643,7 +912,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -651,7 +920,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -659,7 +928,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -667,7 +936,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -675,7 +944,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -683,7 +952,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -691,7 +960,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -699,7 +968,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -707,7 +976,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -715,7 +984,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -723,7 +992,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -731,7 +1000,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -739,7 +1008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -747,7 +1016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -755,7 +1024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -764,14 +1033,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B34">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Wrong Way (One-way)"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:B34"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -780,12 +1049,12 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C12"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -796,7 +1065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -807,7 +1076,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -818,7 +1087,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -829,7 +1098,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -840,7 +1109,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -851,7 +1120,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -862,7 +1131,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -873,7 +1142,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -884,7 +1153,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -895,7 +1164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -906,7 +1175,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -919,6 +1188,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -930,9 +1204,9 @@
       <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -943,7 +1217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -954,7 +1228,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -965,7 +1239,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -976,7 +1250,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -987,7 +1261,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -998,7 +1272,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1009,7 +1283,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1020,7 +1294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1031,7 +1305,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1042,7 +1316,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1053,7 +1327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1066,6 +1340,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1074,15 +1353,15 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C12"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1093,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1104,7 +1383,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1115,7 +1394,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1126,7 +1405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1137,7 +1416,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1148,7 +1427,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1159,7 +1438,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1170,7 +1449,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1181,7 +1460,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1192,7 +1471,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1203,7 +1482,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1216,6 +1495,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1227,14 +1511,14 @@
       <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1256,7 +1540,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1267,7 +1551,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1278,7 +1562,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1289,7 +1573,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1300,7 +1584,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1311,7 +1595,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1322,7 +1606,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1333,7 +1617,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1344,7 +1628,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1355,7 +1639,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1368,6 +1652,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1379,12 +1668,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +1684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1406,7 +1695,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1417,7 +1706,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1428,7 +1717,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1439,7 +1728,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1450,7 +1739,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1461,7 +1750,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1472,7 +1761,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1483,7 +1772,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1494,7 +1783,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1505,7 +1794,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1518,6 +1807,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1527,29 +1821,33 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C282"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C172" sqref="A1:C172"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1560,7 +1858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1571,7 +1869,7 @@
         <v>2727</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1880,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1593,7 +1891,7 @@
         <v>2753</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1604,7 +1902,7 @@
         <v>2454</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1615,7 +1913,7 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1626,7 +1924,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1637,7 +1935,7 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1648,7 +1946,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1659,7 +1957,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +1968,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1681,7 +1979,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1692,7 +1990,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1703,7 +2001,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1714,7 +2012,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1725,7 +2023,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1736,7 +2034,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1747,7 +2045,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1758,7 +2056,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1769,7 +2067,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1780,7 +2078,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1791,7 +2089,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1802,7 +2100,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1813,7 +2111,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1824,7 +2122,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1835,7 +2133,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1846,7 +2144,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1857,7 +2155,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1868,7 +2166,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1879,7 +2177,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1890,7 +2188,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1901,7 +2199,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1912,7 +2210,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1923,7 +2221,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1934,7 +2232,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1945,7 +2243,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1956,7 +2254,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1967,7 +2265,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1978,7 +2276,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1989,7 +2287,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -2000,7 +2298,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2011,7 +2309,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -2022,7 +2320,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -2033,7 +2331,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -2044,7 +2342,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -2055,7 +2353,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2066,7 +2364,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -2077,7 +2375,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2088,7 +2386,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -2099,7 +2397,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -2110,7 +2408,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -2121,7 +2419,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -2132,7 +2430,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -2143,7 +2441,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -2154,7 +2452,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -2165,7 +2463,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -2176,7 +2474,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -2187,7 +2485,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -2198,7 +2496,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -2209,7 +2507,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -2220,7 +2518,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -2231,7 +2529,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -2242,7 +2540,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -2253,7 +2551,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>9</v>
       </c>
@@ -2264,7 +2562,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -2275,7 +2573,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -2286,7 +2584,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -2297,7 +2595,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>9</v>
       </c>
@@ -2308,7 +2606,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>9</v>
       </c>
@@ -2319,7 +2617,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -2330,7 +2628,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -2341,7 +2639,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -2352,7 +2650,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -2363,7 +2661,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -2374,7 +2672,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -2385,7 +2683,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -2396,7 +2694,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -2407,7 +2705,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -2418,7 +2716,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -2429,7 +2727,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -2440,7 +2738,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -2451,7 +2749,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -2462,7 +2760,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -2473,7 +2771,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>9</v>
       </c>
@@ -2484,7 +2782,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>11</v>
       </c>
@@ -2495,7 +2793,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -2506,7 +2804,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>13</v>
       </c>
@@ -2517,7 +2815,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -2528,7 +2826,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -2539,7 +2837,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>13</v>
       </c>
@@ -2550,7 +2848,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>13</v>
       </c>
@@ -2561,7 +2859,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -2572,7 +2870,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>11</v>
       </c>
@@ -2583,7 +2881,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -2594,7 +2892,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -2605,7 +2903,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>10</v>
       </c>
@@ -2616,7 +2914,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -2627,7 +2925,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -2638,7 +2936,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -2649,7 +2947,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -2660,7 +2958,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -2671,7 +2969,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>10</v>
       </c>
@@ -2682,7 +2980,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>14</v>
       </c>
@@ -2693,7 +2991,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>14</v>
       </c>
@@ -2704,7 +3002,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -2715,7 +3013,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>11</v>
       </c>
@@ -2726,7 +3024,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>10</v>
       </c>
@@ -2737,7 +3035,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>12</v>
       </c>
@@ -2748,7 +3046,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -2759,7 +3057,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>15</v>
       </c>
@@ -2770,7 +3068,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>15</v>
       </c>
@@ -2781,7 +3079,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
         <v>8</v>
       </c>
@@ -2792,7 +3090,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
         <v>15</v>
       </c>
@@ -2803,7 +3101,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -2814,7 +3112,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3">
       <c r="A116" t="s">
         <v>12</v>
       </c>
@@ -2825,7 +3123,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3">
       <c r="A117" t="s">
         <v>16</v>
       </c>
@@ -2836,7 +3134,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3">
       <c r="A118" t="s">
         <v>14</v>
       </c>
@@ -2847,7 +3145,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3">
       <c r="A119" t="s">
         <v>11</v>
       </c>
@@ -2858,7 +3156,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3">
       <c r="A120" t="s">
         <v>17</v>
       </c>
@@ -2869,7 +3167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3">
       <c r="A121" t="s">
         <v>15</v>
       </c>
@@ -2880,7 +3178,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3">
       <c r="A122" t="s">
         <v>17</v>
       </c>
@@ -2891,7 +3189,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3">
       <c r="A123" t="s">
         <v>12</v>
       </c>
@@ -2902,7 +3200,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3">
       <c r="A124" t="s">
         <v>15</v>
       </c>
@@ -2913,7 +3211,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3">
       <c r="A125" t="s">
         <v>18</v>
       </c>
@@ -2924,7 +3222,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3">
       <c r="A126" t="s">
         <v>17</v>
       </c>
@@ -2935,7 +3233,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3">
       <c r="A127" t="s">
         <v>15</v>
       </c>
@@ -2946,7 +3244,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3">
       <c r="A128" t="s">
         <v>18</v>
       </c>
@@ -2957,7 +3255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
         <v>14</v>
       </c>
@@ -2968,7 +3266,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -2979,7 +3277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -2990,7 +3288,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3">
       <c r="A132" t="s">
         <v>18</v>
       </c>
@@ -3001,7 +3299,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3">
       <c r="A133" t="s">
         <v>16</v>
       </c>
@@ -3012,7 +3310,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3">
       <c r="A134" t="s">
         <v>16</v>
       </c>
@@ -3023,7 +3321,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3">
       <c r="A135" t="s">
         <v>16</v>
       </c>
@@ -3034,7 +3332,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3">
       <c r="A136" t="s">
         <v>13</v>
       </c>
@@ -3045,7 +3343,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3">
       <c r="A137" t="s">
         <v>16</v>
       </c>
@@ -3056,7 +3354,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3">
       <c r="A138" t="s">
         <v>18</v>
       </c>
@@ -3067,7 +3365,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3">
       <c r="A139" t="s">
         <v>15</v>
       </c>
@@ -3078,7 +3376,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3">
       <c r="A140" t="s">
         <v>12</v>
       </c>
@@ -3089,7 +3387,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3">
       <c r="A141" t="s">
         <v>12</v>
       </c>
@@ -3100,7 +3398,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3">
       <c r="A142" t="s">
         <v>19</v>
       </c>
@@ -3111,7 +3409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3">
       <c r="A143" t="s">
         <v>17</v>
       </c>
@@ -3122,7 +3420,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3">
       <c r="A144" t="s">
         <v>20</v>
       </c>
@@ -3133,7 +3431,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3">
       <c r="A145" t="s">
         <v>15</v>
       </c>
@@ -3144,7 +3442,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3">
       <c r="A146" t="s">
         <v>12</v>
       </c>
@@ -3155,7 +3453,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3">
       <c r="A147" t="s">
         <v>20</v>
       </c>
@@ -3166,7 +3464,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3">
       <c r="A148" t="s">
         <v>19</v>
       </c>
@@ -3177,7 +3475,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3">
       <c r="A149" t="s">
         <v>13</v>
       </c>
@@ -3188,7 +3486,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3">
       <c r="A150" t="s">
         <v>21</v>
       </c>
@@ -3199,7 +3497,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3">
       <c r="A151" t="s">
         <v>15</v>
       </c>
@@ -3210,7 +3508,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3">
       <c r="A152" t="s">
         <v>18</v>
       </c>
@@ -3221,7 +3519,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3">
       <c r="A153" t="s">
         <v>20</v>
       </c>
@@ -3232,7 +3530,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3">
       <c r="A154" t="s">
         <v>15</v>
       </c>
@@ -3243,7 +3541,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3">
       <c r="A155" t="s">
         <v>18</v>
       </c>
@@ -3254,7 +3552,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3">
       <c r="A156" t="s">
         <v>22</v>
       </c>
@@ -3265,7 +3563,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3">
       <c r="A157" t="s">
         <v>13</v>
       </c>
@@ -3276,7 +3574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3">
       <c r="A158" t="s">
         <v>19</v>
       </c>
@@ -3287,7 +3585,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3">
       <c r="A159" t="s">
         <v>18</v>
       </c>
@@ -3298,7 +3596,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3">
       <c r="A160" t="s">
         <v>21</v>
       </c>
@@ -3309,7 +3607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3">
       <c r="A161" t="s">
         <v>16</v>
       </c>
@@ -3320,7 +3618,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3">
       <c r="A162" t="s">
         <v>18</v>
       </c>
@@ -3331,7 +3629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3">
       <c r="A163" t="s">
         <v>18</v>
       </c>
@@ -3342,7 +3640,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3">
       <c r="A164" t="s">
         <v>19</v>
       </c>
@@ -3353,7 +3651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3">
       <c r="A165" t="s">
         <v>19</v>
       </c>
@@ -3364,7 +3662,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3">
       <c r="A166" t="s">
         <v>21</v>
       </c>
@@ -3375,7 +3673,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3">
       <c r="A167" t="s">
         <v>22</v>
       </c>
@@ -3386,7 +3684,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3">
       <c r="A168" t="s">
         <v>19</v>
       </c>
@@ -3397,7 +3695,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3">
       <c r="A169" t="s">
         <v>22</v>
       </c>
@@ -3408,7 +3706,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3">
       <c r="A170" t="s">
         <v>19</v>
       </c>
@@ -3419,7 +3717,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3">
       <c r="A171" t="s">
         <v>16</v>
       </c>
@@ -3430,7 +3728,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3">
       <c r="A172" t="s">
         <v>18</v>
       </c>
@@ -3441,7 +3739,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3">
       <c r="A173" t="s">
         <v>13</v>
       </c>
@@ -3452,7 +3750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3">
       <c r="A174" t="s">
         <v>16</v>
       </c>
@@ -3463,7 +3761,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3">
       <c r="A175" t="s">
         <v>22</v>
       </c>
@@ -3474,7 +3772,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3">
       <c r="A176" t="s">
         <v>23</v>
       </c>
@@ -3485,7 +3783,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3">
       <c r="A177" t="s">
         <v>21</v>
       </c>
@@ -3496,7 +3794,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3">
       <c r="A178" t="s">
         <v>22</v>
       </c>
@@ -3507,7 +3805,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3">
       <c r="A179" t="s">
         <v>16</v>
       </c>
@@ -3518,7 +3816,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3">
       <c r="A180" t="s">
         <v>21</v>
       </c>
@@ -3529,7 +3827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3">
       <c r="A181" t="s">
         <v>20</v>
       </c>
@@ -3540,7 +3838,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3">
       <c r="A182" t="s">
         <v>21</v>
       </c>
@@ -3551,7 +3849,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3">
       <c r="A183" t="s">
         <v>21</v>
       </c>
@@ -3562,7 +3860,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3">
       <c r="A184" t="s">
         <v>24</v>
       </c>
@@ -3573,7 +3871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3">
       <c r="A185" t="s">
         <v>22</v>
       </c>
@@ -3584,7 +3882,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3">
       <c r="A186" t="s">
         <v>13</v>
       </c>
@@ -3595,7 +3893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3">
       <c r="A187" t="s">
         <v>13</v>
       </c>
@@ -3606,7 +3904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3">
       <c r="A188" t="s">
         <v>24</v>
       </c>
@@ -3617,7 +3915,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3">
       <c r="A189" t="s">
         <v>23</v>
       </c>
@@ -3628,7 +3926,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3">
       <c r="A190" t="s">
         <v>21</v>
       </c>
@@ -3639,7 +3937,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3">
       <c r="A191" t="s">
         <v>21</v>
       </c>
@@ -3650,7 +3948,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3">
       <c r="A192" t="s">
         <v>23</v>
       </c>
@@ -3661,7 +3959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3">
       <c r="A193" t="s">
         <v>24</v>
       </c>
@@ -3672,7 +3970,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3">
       <c r="A194" t="s">
         <v>16</v>
       </c>
@@ -3683,7 +3981,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3">
       <c r="A195" t="s">
         <v>22</v>
       </c>
@@ -3694,7 +3992,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3">
       <c r="A196" t="s">
         <v>16</v>
       </c>
@@ -3705,7 +4003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3">
       <c r="A197" t="s">
         <v>24</v>
       </c>
@@ -3716,7 +4014,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3">
       <c r="A198" t="s">
         <v>25</v>
       </c>
@@ -3727,7 +4025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3">
       <c r="A199" t="s">
         <v>19</v>
       </c>
@@ -3738,7 +4036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3">
       <c r="A200" t="s">
         <v>25</v>
       </c>
@@ -3749,7 +4047,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3">
       <c r="A201" t="s">
         <v>26</v>
       </c>
@@ -3760,7 +4058,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3">
       <c r="A202" t="s">
         <v>22</v>
       </c>
@@ -3771,7 +4069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3">
       <c r="A203" t="s">
         <v>22</v>
       </c>
@@ -3782,7 +4080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3">
       <c r="A204" t="s">
         <v>21</v>
       </c>
@@ -3793,7 +4091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3">
       <c r="A205" t="s">
         <v>19</v>
       </c>
@@ -3804,7 +4102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3">
       <c r="A206" t="s">
         <v>19</v>
       </c>
@@ -3815,7 +4113,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3">
       <c r="A207" t="s">
         <v>27</v>
       </c>
@@ -3826,7 +4124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3">
       <c r="A208" t="s">
         <v>28</v>
       </c>
@@ -3837,7 +4135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3">
       <c r="A209" t="s">
         <v>23</v>
       </c>
@@ -3848,7 +4146,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3">
       <c r="A210" t="s">
         <v>28</v>
       </c>
@@ -3859,7 +4157,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3">
       <c r="A211" t="s">
         <v>26</v>
       </c>
@@ -3870,7 +4168,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3">
       <c r="A212" t="s">
         <v>25</v>
       </c>
@@ -3881,7 +4179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3">
       <c r="A213" t="s">
         <v>26</v>
       </c>
@@ -3892,7 +4190,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3">
       <c r="A214" t="s">
         <v>21</v>
       </c>
@@ -3903,7 +4201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3">
       <c r="A215" t="s">
         <v>22</v>
       </c>
@@ -3914,7 +4212,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3">
       <c r="A216" t="s">
         <v>29</v>
       </c>
@@ -3925,7 +4223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3">
       <c r="A217" t="s">
         <v>29</v>
       </c>
@@ -3936,7 +4234,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3">
       <c r="A218" t="s">
         <v>28</v>
       </c>
@@ -3947,7 +4245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3">
       <c r="A219" t="s">
         <v>29</v>
       </c>
@@ -3958,7 +4256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3">
       <c r="A220" t="s">
         <v>28</v>
       </c>
@@ -3969,7 +4267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3">
       <c r="A221" t="s">
         <v>30</v>
       </c>
@@ -3980,7 +4278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3">
       <c r="A222" t="s">
         <v>24</v>
       </c>
@@ -3991,7 +4289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3">
       <c r="A223" t="s">
         <v>24</v>
       </c>
@@ -4002,7 +4300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3">
       <c r="A224" t="s">
         <v>25</v>
       </c>
@@ -4013,7 +4311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3">
       <c r="A225" t="s">
         <v>25</v>
       </c>
@@ -4024,7 +4322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3">
       <c r="A226" t="s">
         <v>26</v>
       </c>
@@ -4035,7 +4333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3">
       <c r="A227" t="s">
         <v>22</v>
       </c>
@@ -4046,7 +4344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="228" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3">
       <c r="A228" t="s">
         <v>25</v>
       </c>
@@ -4057,7 +4355,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="229" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3">
       <c r="A229" t="s">
         <v>19</v>
       </c>
@@ -4068,7 +4366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3">
       <c r="A230" t="s">
         <v>29</v>
       </c>
@@ -4079,7 +4377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="231" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3">
       <c r="A231" t="s">
         <v>30</v>
       </c>
@@ -4090,7 +4388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3">
       <c r="A232" t="s">
         <v>25</v>
       </c>
@@ -4101,7 +4399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="233" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3">
       <c r="A233" t="s">
         <v>30</v>
       </c>
@@ -4112,7 +4410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="234" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3">
       <c r="A234" t="s">
         <v>24</v>
       </c>
@@ -4123,7 +4421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="235" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3">
       <c r="A235" t="s">
         <v>24</v>
       </c>
@@ -4134,7 +4432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="236" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3">
       <c r="A236" t="s">
         <v>25</v>
       </c>
@@ -4145,7 +4443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3">
       <c r="A237" t="s">
         <v>29</v>
       </c>
@@ -4156,7 +4454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="238" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3">
       <c r="A238" t="s">
         <v>31</v>
       </c>
@@ -4167,7 +4465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3">
       <c r="A239" t="s">
         <v>24</v>
       </c>
@@ -4178,7 +4476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3">
       <c r="A240" t="s">
         <v>25</v>
       </c>
@@ -4189,7 +4487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3">
       <c r="A241" t="s">
         <v>30</v>
       </c>
@@ -4200,7 +4498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3">
       <c r="A242" t="s">
         <v>32</v>
       </c>
@@ -4211,7 +4509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3">
       <c r="A243" t="s">
         <v>29</v>
       </c>
@@ -4222,7 +4520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3">
       <c r="A244" t="s">
         <v>24</v>
       </c>
@@ -4233,7 +4531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3">
       <c r="A245" t="s">
         <v>24</v>
       </c>
@@ -4244,7 +4542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3">
       <c r="A246" t="s">
         <v>27</v>
       </c>
@@ -4255,7 +4553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3">
       <c r="A247" t="s">
         <v>31</v>
       </c>
@@ -4266,7 +4564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3">
       <c r="A248" t="s">
         <v>27</v>
       </c>
@@ -4277,7 +4575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3">
       <c r="A249" t="s">
         <v>31</v>
       </c>
@@ -4288,7 +4586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3">
       <c r="A250" t="s">
         <v>27</v>
       </c>
@@ -4299,7 +4597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3">
       <c r="A251" t="s">
         <v>27</v>
       </c>
@@ -4310,7 +4608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3">
       <c r="A252" t="s">
         <v>27</v>
       </c>
@@ -4321,7 +4619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3">
       <c r="A253" t="s">
         <v>27</v>
       </c>
@@ -4332,7 +4630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3">
       <c r="A254" t="s">
         <v>29</v>
       </c>
@@ -4343,7 +4641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3">
       <c r="A255" t="s">
         <v>30</v>
       </c>
@@ -4354,7 +4652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3">
       <c r="A256" t="s">
         <v>32</v>
       </c>
@@ -4365,7 +4663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3">
       <c r="A257" t="s">
         <v>29</v>
       </c>
@@ -4376,7 +4674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3">
       <c r="A258" t="s">
         <v>30</v>
       </c>
@@ -4387,7 +4685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3">
       <c r="A259" t="s">
         <v>30</v>
       </c>
@@ -4398,7 +4696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3">
       <c r="A260" t="s">
         <v>27</v>
       </c>
@@ -4409,7 +4707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3">
       <c r="A261" t="s">
         <v>25</v>
       </c>
@@ -4420,7 +4718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3">
       <c r="A262" t="s">
         <v>27</v>
       </c>
@@ -4431,7 +4729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3">
       <c r="A263" t="s">
         <v>30</v>
       </c>
@@ -4442,7 +4740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3">
       <c r="A264" t="s">
         <v>27</v>
       </c>
@@ -4453,7 +4751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3">
       <c r="A265" t="s">
         <v>29</v>
       </c>
@@ -4464,7 +4762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3">
       <c r="A266" t="s">
         <v>29</v>
       </c>
@@ -4475,7 +4773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3">
       <c r="A267" t="s">
         <v>31</v>
       </c>
@@ -4486,7 +4784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3">
       <c r="A268" t="s">
         <v>29</v>
       </c>
@@ -4497,7 +4795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3">
       <c r="A269" t="s">
         <v>32</v>
       </c>
@@ -4508,7 +4806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3">
       <c r="A270" t="s">
         <v>32</v>
       </c>
@@ -4519,7 +4817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3">
       <c r="A271" t="s">
         <v>30</v>
       </c>
@@ -4530,7 +4828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3">
       <c r="A272" t="s">
         <v>34</v>
       </c>
@@ -4541,7 +4839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3">
       <c r="A273" t="s">
         <v>33</v>
       </c>
@@ -4552,7 +4850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3">
       <c r="A274" t="s">
         <v>25</v>
       </c>
@@ -4563,7 +4861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3">
       <c r="A275" t="s">
         <v>35</v>
       </c>
@@ -4574,7 +4872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3">
       <c r="A276" t="s">
         <v>30</v>
       </c>
@@ -4585,7 +4883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3">
       <c r="A277" t="s">
         <v>27</v>
       </c>
@@ -4596,7 +4894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3">
       <c r="A278" t="s">
         <v>33</v>
       </c>
@@ -4607,7 +4905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3">
       <c r="A279" t="s">
         <v>34</v>
       </c>
@@ -4618,7 +4916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3">
       <c r="A280" t="s">
         <v>34</v>
       </c>
@@ -4629,7 +4927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3">
       <c r="A281" t="s">
         <v>30</v>
       </c>
@@ -4640,7 +4938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3">
       <c r="A282" t="s">
         <v>34</v>
       </c>
@@ -4653,11 +4951,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C282">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Vision Obstructed"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A198:C274">
       <sortCondition ref="B2:B282"/>
     </sortState>
@@ -4666,6 +4959,11 @@
     <sortCondition ref="B2:B172"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4674,17 +4972,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C1" sqref="C1:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4695,7 +4993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4706,7 +5004,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4717,7 +5015,7 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4728,7 +5026,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4739,7 +5037,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -4750,7 +5048,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4761,7 +5059,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -4772,7 +5070,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -4783,7 +5081,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -4794,7 +5092,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -4805,7 +5103,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -4818,6 +5116,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4829,14 +5134,14 @@
       <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4847,7 +5152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4858,7 +5163,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4869,7 +5174,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4880,7 +5185,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -4891,7 +5196,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4902,7 +5207,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4913,7 +5218,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -4924,7 +5229,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -4935,7 +5240,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4946,7 +5251,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -4957,7 +5262,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -4970,6 +5275,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4981,14 +5291,14 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4999,7 +5309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -5010,7 +5320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -5021,7 +5331,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -5032,7 +5342,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -5043,7 +5353,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -5054,7 +5364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -5065,7 +5375,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -5076,7 +5386,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -5087,7 +5397,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -5098,7 +5408,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -5109,7 +5419,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -5122,6 +5432,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5133,14 +5448,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5151,7 +5466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -5162,7 +5477,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -5173,7 +5488,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5184,7 +5499,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -5195,7 +5510,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -5206,7 +5521,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -5217,7 +5532,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -5228,7 +5543,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -5239,7 +5554,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -5250,7 +5565,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5261,7 +5576,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -5274,6 +5589,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5281,13 +5601,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5298,7 +5618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5309,7 +5629,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5320,7 +5640,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -5331,7 +5651,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -5342,7 +5662,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -5353,7 +5673,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -5364,7 +5684,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5375,7 +5695,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -5386,7 +5706,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -5397,7 +5717,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -5408,7 +5728,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -5421,6 +5741,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5432,9 +5757,9 @@
       <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5445,7 +5770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -5456,7 +5781,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -5467,7 +5792,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -5478,7 +5803,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -5489,7 +5814,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -5500,7 +5825,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -5511,7 +5836,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -5522,7 +5847,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -5533,7 +5858,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -5544,7 +5869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -5555,7 +5880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -5568,6 +5893,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5579,9 +5909,9 @@
       <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5592,7 +5922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -5603,7 +5933,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -5614,7 +5944,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -5625,7 +5955,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -5636,7 +5966,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -5647,7 +5977,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -5658,7 +5988,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -5669,7 +5999,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -5680,7 +6010,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5691,7 +6021,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -5702,7 +6032,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -5715,5 +6045,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>